<commit_message>
extended block  + new input functions
</commit_message>
<xml_diff>
--- a/music_database.xlsx
+++ b/music_database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanmaygoel/Documents/GitHub/allisonbot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A645AE1-FD2E-7349-84E5-7F707D5D1F30}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C92AC1B-A05A-D240-AFE9-7E8BEB49EA62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16160" xr2:uid="{CFEADE9C-66A8-F143-95FA-63579C3FB54D}"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16200" xr2:uid="{CFEADE9C-66A8-F143-95FA-63579C3FB54D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>movie</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>sad</t>
+  </si>
+  <si>
+    <t>avengers</t>
   </si>
 </sst>
 </file>
@@ -452,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784B0F75-80E3-0844-8575-C4204C3E9FAB}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -582,6 +585,14 @@
       </c>
       <c r="E7" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fav movie and dataframe integration
</commit_message>
<xml_diff>
--- a/music_database.xlsx
+++ b/music_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanmaygoel/Documents/GitHub/allisonbot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C92AC1B-A05A-D240-AFE9-7E8BEB49EA62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF836D35-DB48-1C4C-B682-A37EA44DACDC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16200" xr2:uid="{CFEADE9C-66A8-F143-95FA-63579C3FB54D}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>movie</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>avengers</t>
+  </si>
+  <si>
+    <t>avengers theme</t>
+  </si>
+  <si>
+    <t>https://youtu.be/FOabQZHT4qY?t=116</t>
   </si>
 </sst>
 </file>
@@ -458,7 +464,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -593,6 +599,15 @@
       </c>
       <c r="B8" t="s">
         <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>